<commit_message>
date format fixed, coach contract added, coach create match checks related to contract time is added , elo change deleted
</commit_message>
<xml_diff>
--- a/chess_db_app/ChessDB_updated.xlsx
+++ b/chess_db_app/ChessDB_updated.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="465">
   <si>
     <t>username</t>
   </si>
@@ -875,412 +875,415 @@
     <t>FIDE043</t>
   </si>
   <si>
+    <t>jamess</t>
+  </si>
+  <si>
+    <t>James!44</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>21-03-1998</t>
+  </si>
+  <si>
+    <t>FIDE044</t>
+  </si>
+  <si>
+    <t>amelia</t>
+  </si>
+  <si>
+    <t>Amelia#99</t>
+  </si>
+  <si>
+    <t>Amelia</t>
+  </si>
+  <si>
+    <t>Zhang</t>
+  </si>
+  <si>
+    <t>FIDE045</t>
+  </si>
+  <si>
+    <t>benjamin</t>
+  </si>
+  <si>
+    <t>Ben@2023</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Fischer</t>
+  </si>
+  <si>
+    <t>27-01-1997</t>
+  </si>
+  <si>
+    <t>FIDE046</t>
+  </si>
+  <si>
+    <t>ella</t>
+  </si>
+  <si>
+    <t>Ella@pw</t>
+  </si>
+  <si>
+    <t>Ella</t>
+  </si>
+  <si>
+    <t>Svensson</t>
+  </si>
+  <si>
+    <t>FIDE047</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t>Alex$88</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Dimitrov</t>
+  </si>
+  <si>
+    <t>BUL</t>
+  </si>
+  <si>
+    <t>22-05-1999</t>
+  </si>
+  <si>
+    <t>FIDE048</t>
+  </si>
+  <si>
+    <t>lily</t>
+  </si>
+  <si>
+    <t>Lily@sun</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Nakamura</t>
+  </si>
+  <si>
+    <t>FIDE049</t>
+  </si>
+  <si>
+    <t>title_name</t>
+  </si>
+  <si>
+    <t>Grandmaster</t>
+  </si>
+  <si>
+    <t>International Master</t>
+  </si>
+  <si>
+    <t>FIDE Master</t>
+  </si>
+  <si>
+    <t>Candidate Master</t>
+  </si>
+  <si>
+    <t>National Master</t>
+  </si>
+  <si>
+    <t>team_id</t>
+  </si>
+  <si>
+    <t>contract_start</t>
+  </si>
+  <si>
+    <t>contract_finish</t>
+  </si>
+  <si>
+    <t>carol</t>
+  </si>
+  <si>
+    <t>coachpw</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>david_b</t>
+  </si>
+  <si>
+    <t>dPass!99</t>
+  </si>
+  <si>
+    <t>15-02-2024</t>
+  </si>
+  <si>
+    <t>15-02-2026</t>
+  </si>
+  <si>
+    <t>emma_green</t>
+  </si>
+  <si>
+    <t>E@mma77</t>
+  </si>
+  <si>
+    <t>fatih</t>
+  </si>
+  <si>
+    <t>FatihC21</t>
+  </si>
+  <si>
+    <t>Fatih</t>
+  </si>
+  <si>
+    <t>Ceylan</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>hana</t>
+  </si>
+  <si>
+    <t>Hana$45</t>
+  </si>
+  <si>
+    <t>Hana</t>
+  </si>
+  <si>
+    <t>Yamada</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>lucaas</t>
+  </si>
+  <si>
+    <t>Lucas#1</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>mia_rose</t>
+  </si>
+  <si>
+    <t>Mia!888</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>onur</t>
+  </si>
+  <si>
+    <t>onUr@32</t>
+  </si>
+  <si>
+    <t>Onur</t>
+  </si>
+  <si>
+    <t>Kaya</t>
+  </si>
+  <si>
+    <t>15-03-2023</t>
+  </si>
+  <si>
+    <t>15-09-2025</t>
+  </si>
+  <si>
+    <t>sofia_lop</t>
+  </si>
+  <si>
+    <t>S0fia#</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>arslan_yusuf</t>
+  </si>
+  <si>
+    <t>Yusuf199</t>
+  </si>
+  <si>
+    <t>Arslan</t>
+  </si>
+  <si>
+    <t>coach_username</t>
+  </si>
+  <si>
+    <t>certification</t>
+  </si>
+  <si>
+    <t>FIDE Certified</t>
+  </si>
+  <si>
+    <t>National Level</t>
+  </si>
+  <si>
+    <t>Regional Certified</t>
+  </si>
+  <si>
+    <t>Club Level</t>
+  </si>
+  <si>
+    <t>team_name</t>
+  </si>
+  <si>
+    <t>sponsor_id</t>
+  </si>
+  <si>
+    <t>Knights</t>
+  </si>
+  <si>
+    <t>Rooks</t>
+  </si>
+  <si>
+    <t>Bishops</t>
+  </si>
+  <si>
+    <t>Pawns</t>
+  </si>
+  <si>
+    <t>Queens</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Castles</t>
+  </si>
+  <si>
+    <t>Checkmates</t>
+  </si>
+  <si>
+    <t>En Passants</t>
+  </si>
+  <si>
+    <t>Blitz Masters</t>
+  </si>
+  <si>
+    <t>sponsor_name</t>
+  </si>
+  <si>
+    <t>ChessVision</t>
+  </si>
+  <si>
+    <t>Grandmaster Corp</t>
+  </si>
+  <si>
+    <t>Queen’s Gambit Ltd.</t>
+  </si>
+  <si>
+    <t>MateMate Inc.</t>
+  </si>
+  <si>
+    <t>RookTech</t>
+  </si>
+  <si>
+    <t>PawnPower Solutions</t>
+  </si>
+  <si>
+    <t>CheckSecure AG</t>
+  </si>
+  <si>
+    <t>Endgame Enterprises</t>
+  </si>
+  <si>
+    <t>King's Arena Foundation</t>
+  </si>
+  <si>
+    <t>experience_level</t>
+  </si>
+  <si>
+    <t>erin</t>
+  </si>
+  <si>
+    <t>arbpw</t>
+  </si>
+  <si>
+    <t>Erin</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>refpass</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Blake</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>lucy</t>
+  </si>
+  <si>
+    <t>arb123</t>
+  </si>
+  <si>
+    <t>Lucy</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>ahmet</t>
+  </si>
+  <si>
+    <t>pass2024</t>
+  </si>
+  <si>
+    <t>Ahmet</t>
+  </si>
+  <si>
+    <t>Yılmaz</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>ana</t>
+  </si>
+  <si>
+    <t>secretpw</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Costa</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
     <t>james</t>
-  </si>
-  <si>
-    <t>James!44</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>21-03-1998</t>
-  </si>
-  <si>
-    <t>FIDE044</t>
-  </si>
-  <si>
-    <t>amelia</t>
-  </si>
-  <si>
-    <t>Amelia#99</t>
-  </si>
-  <si>
-    <t>Amelia</t>
-  </si>
-  <si>
-    <t>Zhang</t>
-  </si>
-  <si>
-    <t>FIDE045</t>
-  </si>
-  <si>
-    <t>benjamin</t>
-  </si>
-  <si>
-    <t>Ben@2023</t>
-  </si>
-  <si>
-    <t>Benjamin</t>
-  </si>
-  <si>
-    <t>Fischer</t>
-  </si>
-  <si>
-    <t>27-01-1997</t>
-  </si>
-  <si>
-    <t>FIDE046</t>
-  </si>
-  <si>
-    <t>ella</t>
-  </si>
-  <si>
-    <t>Ella@pw</t>
-  </si>
-  <si>
-    <t>Ella</t>
-  </si>
-  <si>
-    <t>Svensson</t>
-  </si>
-  <si>
-    <t>FIDE047</t>
-  </si>
-  <si>
-    <t>alex</t>
-  </si>
-  <si>
-    <t>Alex$88</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Dimitrov</t>
-  </si>
-  <si>
-    <t>BUL</t>
-  </si>
-  <si>
-    <t>22-05-1999</t>
-  </si>
-  <si>
-    <t>FIDE048</t>
-  </si>
-  <si>
-    <t>lily</t>
-  </si>
-  <si>
-    <t>Lily@sun</t>
-  </si>
-  <si>
-    <t>Lily</t>
-  </si>
-  <si>
-    <t>Nakamura</t>
-  </si>
-  <si>
-    <t>FIDE049</t>
-  </si>
-  <si>
-    <t>title_name</t>
-  </si>
-  <si>
-    <t>Grandmaster</t>
-  </si>
-  <si>
-    <t>International Master</t>
-  </si>
-  <si>
-    <t>FIDE Master</t>
-  </si>
-  <si>
-    <t>Candidate Master</t>
-  </si>
-  <si>
-    <t>National Master</t>
-  </si>
-  <si>
-    <t>team_id</t>
-  </si>
-  <si>
-    <t>contract_start</t>
-  </si>
-  <si>
-    <t>contract_finish</t>
-  </si>
-  <si>
-    <t>carol</t>
-  </si>
-  <si>
-    <t>coachpw</t>
-  </si>
-  <si>
-    <t>Carol</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>david_b</t>
-  </si>
-  <si>
-    <t>dPass!99</t>
-  </si>
-  <si>
-    <t>15-02-2024</t>
-  </si>
-  <si>
-    <t>15-02-2026</t>
-  </si>
-  <si>
-    <t>emma_green</t>
-  </si>
-  <si>
-    <t>E@mma77</t>
-  </si>
-  <si>
-    <t>fatih</t>
-  </si>
-  <si>
-    <t>FatihC21</t>
-  </si>
-  <si>
-    <t>Fatih</t>
-  </si>
-  <si>
-    <t>Ceylan</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>hana</t>
-  </si>
-  <si>
-    <t>Hana$45</t>
-  </si>
-  <si>
-    <t>Hana</t>
-  </si>
-  <si>
-    <t>Yamada</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>lucaas</t>
-  </si>
-  <si>
-    <t>Lucas#1</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>mia_rose</t>
-  </si>
-  <si>
-    <t>Mia!888</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>onur</t>
-  </si>
-  <si>
-    <t>onUr@32</t>
-  </si>
-  <si>
-    <t>Onur</t>
-  </si>
-  <si>
-    <t>Kaya</t>
-  </si>
-  <si>
-    <t>15-03-2023</t>
-  </si>
-  <si>
-    <t>15-09-2025</t>
-  </si>
-  <si>
-    <t>sofia_lop</t>
-  </si>
-  <si>
-    <t>S0fia#</t>
-  </si>
-  <si>
-    <t>López</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>arslan_yusuf</t>
-  </si>
-  <si>
-    <t>Yusuf199</t>
-  </si>
-  <si>
-    <t>Arslan</t>
-  </si>
-  <si>
-    <t>coach_username</t>
-  </si>
-  <si>
-    <t>certification</t>
-  </si>
-  <si>
-    <t>FIDE Certified</t>
-  </si>
-  <si>
-    <t>National Level</t>
-  </si>
-  <si>
-    <t>Regional Certified</t>
-  </si>
-  <si>
-    <t>Club Level</t>
-  </si>
-  <si>
-    <t>team_name</t>
-  </si>
-  <si>
-    <t>sponsor_id</t>
-  </si>
-  <si>
-    <t>Knights</t>
-  </si>
-  <si>
-    <t>Rooks</t>
-  </si>
-  <si>
-    <t>Bishops</t>
-  </si>
-  <si>
-    <t>Pawns</t>
-  </si>
-  <si>
-    <t>Queens</t>
-  </si>
-  <si>
-    <t>Kings</t>
-  </si>
-  <si>
-    <t>Castles</t>
-  </si>
-  <si>
-    <t>Checkmates</t>
-  </si>
-  <si>
-    <t>En Passants</t>
-  </si>
-  <si>
-    <t>Blitz Masters</t>
-  </si>
-  <si>
-    <t>sponsor_name</t>
-  </si>
-  <si>
-    <t>ChessVision</t>
-  </si>
-  <si>
-    <t>Grandmaster Corp</t>
-  </si>
-  <si>
-    <t>Queen’s Gambit Ltd.</t>
-  </si>
-  <si>
-    <t>MateMate Inc.</t>
-  </si>
-  <si>
-    <t>RookTech</t>
-  </si>
-  <si>
-    <t>PawnPower Solutions</t>
-  </si>
-  <si>
-    <t>CheckSecure AG</t>
-  </si>
-  <si>
-    <t>Endgame Enterprises</t>
-  </si>
-  <si>
-    <t>King's Arena Foundation</t>
-  </si>
-  <si>
-    <t>experience_level</t>
-  </si>
-  <si>
-    <t>erin</t>
-  </si>
-  <si>
-    <t>arbpw</t>
-  </si>
-  <si>
-    <t>Erin</t>
-  </si>
-  <si>
-    <t>Gray</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>mark</t>
-  </si>
-  <si>
-    <t>refpass</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Blake</t>
-  </si>
-  <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
-    <t>lucy</t>
-  </si>
-  <si>
-    <t>arb123</t>
-  </si>
-  <si>
-    <t>Lucy</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>ahmet</t>
-  </si>
-  <si>
-    <t>pass2024</t>
-  </si>
-  <si>
-    <t>Ahmet</t>
-  </si>
-  <si>
-    <t>Yılmaz</t>
-  </si>
-  <si>
-    <t>Beginner</t>
-  </si>
-  <si>
-    <t>ana</t>
-  </si>
-  <si>
-    <t>secretpw</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>Costa</t>
-  </si>
-  <si>
-    <t>Brazil</t>
   </si>
   <si>
     <t>secure1</t>
@@ -29904,7 +29907,7 @@
         <v>399</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4">
@@ -29912,7 +29915,7 @@
         <v>404</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5">
@@ -29920,7 +29923,7 @@
         <v>409</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6">
@@ -29933,26 +29936,26 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>283</v>
+        <v>419</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -29975,16 +29978,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
@@ -29992,7 +29995,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -30006,7 +30009,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
@@ -30020,7 +30023,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>348</v>
@@ -30034,7 +30037,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>340</v>
@@ -30048,10 +30051,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D6" s="3">
         <v>9.0</v>
@@ -30062,7 +30065,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>361</v>
@@ -30076,7 +30079,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>351</v>
@@ -30090,10 +30093,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D9" s="3">
         <v>8.0</v>
@@ -30104,7 +30107,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>329</v>
@@ -30118,7 +30121,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>345</v>
@@ -30144,10 +30147,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="2">
@@ -30298,31 +30301,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>449</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2">
@@ -30394,10 +30397,10 @@
         <v>1.0</v>
       </c>
       <c r="D4" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" s="3">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F4" s="3">
         <v>5.0</v>
@@ -30409,7 +30412,7 @@
         <v>399</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="5">
@@ -30426,7 +30429,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="3">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F5" s="3">
         <v>7.0</v>
@@ -30452,10 +30455,10 @@
         <v>1.0</v>
       </c>
       <c r="D6" s="3">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E6" s="3">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="F6" s="3">
         <v>9.0</v>
@@ -30467,7 +30470,7 @@
         <v>404</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7">
@@ -30484,7 +30487,7 @@
         <v>3.0</v>
       </c>
       <c r="E7" s="3">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="F7" s="3">
         <v>1.0</v>
@@ -30493,10 +30496,10 @@
         <v>3.0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8">
@@ -30510,10 +30513,10 @@
         <v>1.0</v>
       </c>
       <c r="D8" s="3">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E8" s="3">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="F8" s="3">
         <v>2.0</v>
@@ -30539,10 +30542,10 @@
         <v>3.0</v>
       </c>
       <c r="D9" s="3">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E9" s="3">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="F9" s="3">
         <v>6.0</v>
@@ -30551,7 +30554,7 @@
         <v>7.0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I9" s="3">
         <v>3.1</v>
@@ -30568,10 +30571,10 @@
         <v>1.0</v>
       </c>
       <c r="D10" s="3">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E10" s="3">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="F10" s="3">
         <v>8.0</v>
@@ -30600,7 +30603,7 @@
         <v>5.0</v>
       </c>
       <c r="E11" s="3">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="F11" s="3">
         <v>10.0</v>
@@ -30626,10 +30629,10 @@
         <v>1.0</v>
       </c>
       <c r="D12" s="3">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="E12" s="3">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="F12" s="3">
         <v>3.0</v>
@@ -30638,7 +30641,7 @@
         <v>5.0</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>283</v>
+        <v>419</v>
       </c>
       <c r="I12" s="3">
         <v>5.1</v>
@@ -30655,10 +30658,10 @@
         <v>3.0</v>
       </c>
       <c r="D13" s="3">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="E13" s="3">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="F13" s="3">
         <v>4.0</v>
@@ -30670,7 +30673,7 @@
         <v>404</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14">
@@ -30684,10 +30687,10 @@
         <v>1.0</v>
       </c>
       <c r="D14" s="3">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="E14" s="3">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F14" s="3">
         <v>7.0</v>
@@ -30696,10 +30699,10 @@
         <v>9.0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15">
@@ -30713,10 +30716,10 @@
         <v>3.0</v>
       </c>
       <c r="D15" s="3">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="E15" s="3">
-        <v>2.0</v>
+        <v>14.0</v>
       </c>
       <c r="F15" s="3">
         <v>8.0</v>
@@ -30725,7 +30728,7 @@
         <v>10.0</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I15" s="3">
         <v>2.6</v>
@@ -30742,10 +30745,10 @@
         <v>1.0</v>
       </c>
       <c r="D16" s="3">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
       <c r="E16" s="3">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="F16" s="3">
         <v>1.0</v>
@@ -30771,10 +30774,10 @@
         <v>3.0</v>
       </c>
       <c r="D17" s="3">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="E17" s="3">
-        <v>2.0</v>
+        <v>16.0</v>
       </c>
       <c r="F17" s="3">
         <v>2.0</v>
@@ -30800,10 +30803,10 @@
         <v>1.0</v>
       </c>
       <c r="D18" s="3">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
       <c r="E18" s="3">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="F18" s="3">
         <v>3.0</v>
@@ -30812,10 +30815,10 @@
         <v>6.0</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>283</v>
+        <v>419</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19">
@@ -30829,10 +30832,10 @@
         <v>3.0</v>
       </c>
       <c r="D19" s="3">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="E19" s="3">
-        <v>2.0</v>
+        <v>14.0</v>
       </c>
       <c r="F19" s="3">
         <v>7.0</v>
@@ -30858,10 +30861,10 @@
         <v>1.0</v>
       </c>
       <c r="D20" s="3">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="E20" s="3">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="F20" s="3">
         <v>5.0</v>
@@ -30887,10 +30890,10 @@
         <v>3.0</v>
       </c>
       <c r="D21" s="3">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="E21" s="3">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="F21" s="3">
         <v>6.0</v>
@@ -30922,16 +30925,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2">
@@ -30945,7 +30948,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3">
@@ -30959,7 +30962,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4">
@@ -30973,7 +30976,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5">
@@ -30987,7 +30990,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6">
@@ -31001,7 +31004,7 @@
         <v>83</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7">
@@ -31015,7 +31018,7 @@
         <v>94</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8">
@@ -31029,7 +31032,7 @@
         <v>107</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9">
@@ -31043,7 +31046,7 @@
         <v>117</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10">
@@ -31057,7 +31060,7 @@
         <v>129</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11">
@@ -31071,7 +31074,7 @@
         <v>142</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12">
@@ -31085,7 +31088,7 @@
         <v>148</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13">
@@ -31099,7 +31102,7 @@
         <v>154</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="14">
@@ -31113,7 +31116,7 @@
         <v>161</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="15">
@@ -31127,7 +31130,7 @@
         <v>168</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="16">
@@ -31141,7 +31144,7 @@
         <v>174</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="17">
@@ -31155,7 +31158,7 @@
         <v>180</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18">
@@ -31169,7 +31172,7 @@
         <v>186</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19">
@@ -31183,7 +31186,7 @@
         <v>192</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20">
@@ -31197,7 +31200,7 @@
         <v>198</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21">
@@ -31211,7 +31214,7 @@
         <v>204</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -40957,10 +40960,10 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>283</v>
+        <v>419</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>285</v>
@@ -40977,19 +40980,19 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>408</v>
@@ -40997,19 +41000,19 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>398</v>

</xml_diff>